<commit_message>
Various changes, mostly to Using R for Analysis slides.
</commit_message>
<xml_diff>
--- a/output/Tool-Comparison.xlsx
+++ b/output/Tool-Comparison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="25200" windowHeight="12435"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="25200" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
   <si>
     <t>Excel</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>workflow flexibility</t>
+  </si>
+  <si>
+    <t>adsf</t>
   </si>
 </sst>
 </file>
@@ -202,8 +205,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D12" totalsRowShown="0">
-  <autoFilter ref="A1:D12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:E12" totalsRowShown="0">
+  <autoFilter ref="B1:E12"/>
   <tableColumns count="4">
     <tableColumn id="1" name="task"/>
     <tableColumn id="2" name="Excel" dataDxfId="7"/>
@@ -477,190 +480,195 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="B1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="E8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:D12">
+  <conditionalFormatting sqref="C2:E12">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"meh"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updates for fall 2018
</commit_message>
<xml_diff>
--- a/output/Tool-Comparison.xlsx
+++ b/output/Tool-Comparison.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtolbert\Desktop\airline-is470-class\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ALUMNI\Jake T\Presentations\airline-is470-class\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="25200" windowHeight="12435"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="25200" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="20">
   <si>
     <t>Excel</t>
   </si>
@@ -50,9 +50,6 @@
     <t>best</t>
   </si>
   <si>
-    <t>update data</t>
-  </si>
-  <si>
     <t>reproducible analysis</t>
   </si>
   <si>
@@ -83,10 +80,10 @@
     <t>capabilities</t>
   </si>
   <si>
-    <t>workflow flexibility</t>
-  </si>
-  <si>
-    <t>adsf</t>
+    <t>separate data &amp; analysis</t>
+  </si>
+  <si>
+    <t>data exploration</t>
   </si>
 </sst>
 </file>
@@ -133,6 +130,15 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color theme="0"/>
       </font>
@@ -176,15 +182,6 @@
       <font>
         <color theme="1" tint="0.499984740745262"/>
       </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -209,9 +206,9 @@
   <autoFilter ref="B1:E12"/>
   <tableColumns count="4">
     <tableColumn id="1" name="task"/>
-    <tableColumn id="2" name="Excel" dataDxfId="7"/>
-    <tableColumn id="3" name="QlikView" dataDxfId="6"/>
-    <tableColumn id="4" name="R" dataDxfId="5"/>
+    <tableColumn id="2" name="Excel" dataDxfId="2"/>
+    <tableColumn id="3" name="QlikView" dataDxfId="1"/>
+    <tableColumn id="4" name="R" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -480,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E16"/>
+  <dimension ref="B1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +521,7 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
@@ -538,16 +535,16 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -561,18 +558,18 @@
         <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>7</v>
@@ -580,13 +577,13 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
@@ -594,27 +591,27 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>7</v>
@@ -622,7 +619,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
@@ -631,26 +628,26 @@
         <v>6</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>7</v>
@@ -659,29 +656,24 @@
         <v>6</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:E12">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"meh"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"bad"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"good"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"best"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"awful"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>